<commit_message>
Updating drivers to fix a few bugs
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\220038920\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F33D75-F61F-45DC-9CA6-8FA74A46E4BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7639F1-D60D-420F-9B2D-9B7466CCCB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
   </bookViews>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="226">
   <si>
     <t>Device</t>
   </si>
@@ -691,6 +694,27 @@
   </si>
   <si>
     <t>10.2.0.179</t>
+  </si>
+  <si>
+    <t>Chamber 1 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 2 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 3 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 4 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 5 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 6 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 7 Environmental</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6BCF3-52DA-45D5-A06F-31378179F4D8}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="H242" sqref="H242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6649,100 +6673,135 @@
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D245">
-        <v>10</v>
-      </c>
-      <c r="E245">
-        <v>2</v>
-      </c>
-      <c r="F245">
-        <v>0</v>
-      </c>
-      <c r="G245">
+      <c r="A245" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B245" s="3"/>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3">
+        <v>10</v>
+      </c>
+      <c r="E245" s="3">
+        <v>2</v>
+      </c>
+      <c r="F245" s="3">
+        <v>0</v>
+      </c>
+      <c r="G245" s="3">
         <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D246">
-        <v>10</v>
-      </c>
-      <c r="E246">
-        <v>2</v>
-      </c>
-      <c r="F246">
-        <v>0</v>
-      </c>
-      <c r="G246">
+      <c r="A246" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B246" s="3"/>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3">
+        <v>10</v>
+      </c>
+      <c r="E246" s="3">
+        <v>2</v>
+      </c>
+      <c r="F246" s="3">
+        <v>0</v>
+      </c>
+      <c r="G246" s="3">
         <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D247">
-        <v>10</v>
-      </c>
-      <c r="E247">
-        <v>2</v>
-      </c>
-      <c r="F247">
-        <v>0</v>
-      </c>
-      <c r="G247">
+      <c r="A247" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B247" s="3"/>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3">
+        <v>10</v>
+      </c>
+      <c r="E247" s="3">
+        <v>2</v>
+      </c>
+      <c r="F247" s="3">
+        <v>0</v>
+      </c>
+      <c r="G247" s="3">
         <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D248">
-        <v>10</v>
-      </c>
-      <c r="E248">
-        <v>2</v>
-      </c>
-      <c r="F248">
-        <v>0</v>
-      </c>
-      <c r="G248">
+      <c r="A248" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B248" s="3"/>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3">
+        <v>10</v>
+      </c>
+      <c r="E248" s="3">
+        <v>2</v>
+      </c>
+      <c r="F248" s="3">
+        <v>0</v>
+      </c>
+      <c r="G248" s="3">
         <v>247</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D249">
-        <v>10</v>
-      </c>
-      <c r="E249">
-        <v>2</v>
-      </c>
-      <c r="F249">
-        <v>0</v>
-      </c>
-      <c r="G249">
+      <c r="A249" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B249" s="3"/>
+      <c r="C249" s="3"/>
+      <c r="D249" s="3">
+        <v>10</v>
+      </c>
+      <c r="E249" s="3">
+        <v>2</v>
+      </c>
+      <c r="F249" s="3">
+        <v>0</v>
+      </c>
+      <c r="G249" s="3">
         <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D250">
-        <v>10</v>
-      </c>
-      <c r="E250">
-        <v>2</v>
-      </c>
-      <c r="F250">
-        <v>0</v>
-      </c>
-      <c r="G250">
+      <c r="A250" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="B250" s="3"/>
+      <c r="C250" s="3"/>
+      <c r="D250" s="3">
+        <v>10</v>
+      </c>
+      <c r="E250" s="3">
+        <v>2</v>
+      </c>
+      <c r="F250" s="3">
+        <v>0</v>
+      </c>
+      <c r="G250" s="3">
         <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D251">
-        <v>10</v>
-      </c>
-      <c r="E251">
-        <v>2</v>
-      </c>
-      <c r="F251">
-        <v>0</v>
-      </c>
-      <c r="G251">
+      <c r="A251" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3">
+        <v>10</v>
+      </c>
+      <c r="E251" s="3">
+        <v>2</v>
+      </c>
+      <c r="F251" s="3">
+        <v>0</v>
+      </c>
+      <c r="G251" s="3">
         <v>250</v>
       </c>
     </row>
@@ -6834,5 +6893,6 @@
     <mergeCell ref="B218:B219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing the UEF and FHR tests. updated PID and improved last second decision for FHR
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EF4021-B652-4EAD-B20A-F91C14F09961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC0A55D-DF83-4090-A6E7-2EB8A69B84BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
   </bookViews>
@@ -573,214 +573,214 @@
     <t>10.2.0.197</t>
   </si>
   <si>
+    <t>10.2.0.200</t>
+  </si>
+  <si>
+    <t>10.2.0.201</t>
+  </si>
+  <si>
+    <t>10.2.0.202</t>
+  </si>
+  <si>
+    <t>10.2.0.203</t>
+  </si>
+  <si>
+    <t>10.2.0.205</t>
+  </si>
+  <si>
+    <t>10.2.0.206</t>
+  </si>
+  <si>
+    <t>10.2.0.207</t>
+  </si>
+  <si>
+    <t>10.2.0.208</t>
+  </si>
+  <si>
+    <t>PRAT 1</t>
+  </si>
+  <si>
+    <t>10.2.1.11</t>
+  </si>
+  <si>
+    <t>IP Free</t>
+  </si>
+  <si>
+    <t>10.2.0.210</t>
+  </si>
+  <si>
+    <t>PRAT 2</t>
+  </si>
+  <si>
+    <t>10.2.0.212</t>
+  </si>
+  <si>
+    <t>PRAT 3</t>
+  </si>
+  <si>
+    <t>10.2.0.214</t>
+  </si>
+  <si>
+    <t>PRAT 4</t>
+  </si>
+  <si>
+    <t>10.2.0.216</t>
+  </si>
+  <si>
+    <t>PRAT 5</t>
+  </si>
+  <si>
+    <t>10.2.0.218</t>
+  </si>
+  <si>
+    <t>PRAT 6</t>
+  </si>
+  <si>
+    <t>10.2.0.220</t>
+  </si>
+  <si>
+    <t>PRAT 7</t>
+  </si>
+  <si>
+    <t>10.2.0.222</t>
+  </si>
+  <si>
+    <t>PRAT 8</t>
+  </si>
+  <si>
+    <t>10.2.0.224</t>
+  </si>
+  <si>
+    <t>Zoneline Computer 1</t>
+  </si>
+  <si>
+    <t>10.2.0.226</t>
+  </si>
+  <si>
+    <t>Zoneline Computer 2</t>
+  </si>
+  <si>
+    <t>10.2.0.227</t>
+  </si>
+  <si>
+    <t>Zoneline Computer 3</t>
+  </si>
+  <si>
+    <t>10.2.0.228</t>
+  </si>
+  <si>
+    <t>3 ED</t>
+  </si>
+  <si>
+    <t>4 ED</t>
+  </si>
+  <si>
+    <t>4ED</t>
+  </si>
+  <si>
+    <t>Network Broadcast Address</t>
+  </si>
+  <si>
+    <t>10.2.0.79</t>
+  </si>
+  <si>
+    <t>10.2.0.173</t>
+  </si>
+  <si>
+    <t>10.2.0.179</t>
+  </si>
+  <si>
+    <t>Chamber 1 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 2 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 3 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 4 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 5 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 6 Environmental</t>
+  </si>
+  <si>
+    <t>Chamber 7 Environmental</t>
+  </si>
+  <si>
+    <t>FVIR Water Flow Meter</t>
+  </si>
+  <si>
+    <t>LDO Water Flow Meter</t>
+  </si>
+  <si>
+    <t>EtherNet/IP Adapter 1734-AENTR</t>
+  </si>
+  <si>
+    <t>EtherNet/IP Adapter 1719-AENTR EX</t>
+  </si>
+  <si>
+    <t>Anybus X-gateway EtherNet/IP-Modbus TCP</t>
+  </si>
+  <si>
+    <t>Allen Bradley Compact Logic 5380</t>
+  </si>
+  <si>
+    <t>Computer PC with LabView/Studio 5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FV ICPCON 7188E8 RS232 Gateway	</t>
+  </si>
+  <si>
+    <t>LDO ICPCON 7188E8 RS232 Gateway</t>
+  </si>
+  <si>
+    <t>10.2.0.9</t>
+  </si>
+  <si>
+    <t>10.2.0.10</t>
+  </si>
+  <si>
+    <t>10.2.0.11</t>
+  </si>
+  <si>
+    <t>10.2.0.12</t>
+  </si>
+  <si>
+    <t>10.2.0.13</t>
+  </si>
+  <si>
+    <t>10.2.0.14</t>
+  </si>
+  <si>
+    <t>10.2.0.15</t>
+  </si>
+  <si>
+    <t>10.2.0.16</t>
+  </si>
+  <si>
+    <t>10.2.0.17</t>
+  </si>
+  <si>
+    <t>10.2.0.18</t>
+  </si>
+  <si>
+    <t>10.2.0.19</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>FVIR</t>
+  </si>
+  <si>
+    <t>FVIR &amp; LDO</t>
+  </si>
+  <si>
     <t>10.2.0.198</t>
-  </si>
-  <si>
-    <t>10.2.0.200</t>
-  </si>
-  <si>
-    <t>10.2.0.201</t>
-  </si>
-  <si>
-    <t>10.2.0.202</t>
-  </si>
-  <si>
-    <t>10.2.0.203</t>
-  </si>
-  <si>
-    <t>10.2.0.205</t>
-  </si>
-  <si>
-    <t>10.2.0.206</t>
-  </si>
-  <si>
-    <t>10.2.0.207</t>
-  </si>
-  <si>
-    <t>10.2.0.208</t>
-  </si>
-  <si>
-    <t>PRAT 1</t>
-  </si>
-  <si>
-    <t>10.2.1.11</t>
-  </si>
-  <si>
-    <t>IP Free</t>
-  </si>
-  <si>
-    <t>10.2.0.210</t>
-  </si>
-  <si>
-    <t>PRAT 2</t>
-  </si>
-  <si>
-    <t>10.2.0.212</t>
-  </si>
-  <si>
-    <t>PRAT 3</t>
-  </si>
-  <si>
-    <t>10.2.0.214</t>
-  </si>
-  <si>
-    <t>PRAT 4</t>
-  </si>
-  <si>
-    <t>10.2.0.216</t>
-  </si>
-  <si>
-    <t>PRAT 5</t>
-  </si>
-  <si>
-    <t>10.2.0.218</t>
-  </si>
-  <si>
-    <t>PRAT 6</t>
-  </si>
-  <si>
-    <t>10.2.0.220</t>
-  </si>
-  <si>
-    <t>PRAT 7</t>
-  </si>
-  <si>
-    <t>10.2.0.222</t>
-  </si>
-  <si>
-    <t>PRAT 8</t>
-  </si>
-  <si>
-    <t>10.2.0.224</t>
-  </si>
-  <si>
-    <t>Zoneline Computer 1</t>
-  </si>
-  <si>
-    <t>10.2.0.226</t>
-  </si>
-  <si>
-    <t>Zoneline Computer 2</t>
-  </si>
-  <si>
-    <t>10.2.0.227</t>
-  </si>
-  <si>
-    <t>Zoneline Computer 3</t>
-  </si>
-  <si>
-    <t>10.2.0.228</t>
-  </si>
-  <si>
-    <t>3 ED</t>
-  </si>
-  <si>
-    <t>4 ED</t>
-  </si>
-  <si>
-    <t>4ED</t>
-  </si>
-  <si>
-    <t>Network Broadcast Address</t>
-  </si>
-  <si>
-    <t>10.2.0.79</t>
-  </si>
-  <si>
-    <t>10.2.0.173</t>
-  </si>
-  <si>
-    <t>10.2.0.179</t>
-  </si>
-  <si>
-    <t>Chamber 1 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 2 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 3 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 4 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 5 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 6 Environmental</t>
-  </si>
-  <si>
-    <t>Chamber 7 Environmental</t>
-  </si>
-  <si>
-    <t>FVIR Water Flow Meter</t>
-  </si>
-  <si>
-    <t>LDO Water Flow Meter</t>
-  </si>
-  <si>
-    <t>EtherNet/IP Adapter 1734-AENTR</t>
-  </si>
-  <si>
-    <t>EtherNet/IP Adapter 1719-AENTR EX</t>
-  </si>
-  <si>
-    <t>Anybus X-gateway EtherNet/IP-Modbus TCP</t>
-  </si>
-  <si>
-    <t>Allen Bradley Compact Logic 5380</t>
-  </si>
-  <si>
-    <t>Computer PC with LabView/Studio 5000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FV ICPCON 7188E8 RS232 Gateway	</t>
-  </si>
-  <si>
-    <t>LDO ICPCON 7188E8 RS232 Gateway</t>
-  </si>
-  <si>
-    <t>10.2.0.9</t>
-  </si>
-  <si>
-    <t>10.2.0.10</t>
-  </si>
-  <si>
-    <t>10.2.0.11</t>
-  </si>
-  <si>
-    <t>10.2.0.12</t>
-  </si>
-  <si>
-    <t>10.2.0.13</t>
-  </si>
-  <si>
-    <t>10.2.0.14</t>
-  </si>
-  <si>
-    <t>10.2.0.15</t>
-  </si>
-  <si>
-    <t>10.2.0.16</t>
-  </si>
-  <si>
-    <t>10.2.0.17</t>
-  </si>
-  <si>
-    <t>10.2.0.18</t>
-  </si>
-  <si>
-    <t>10.2.0.19</t>
-  </si>
-  <si>
-    <t>LDO</t>
-  </si>
-  <si>
-    <t>FVIR</t>
-  </si>
-  <si>
-    <t>FVIR &amp; LDO</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,6 +930,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1395,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6BCF3-52DA-45D5-A06F-31378179F4D8}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,13 +1742,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D10" s="20">
         <v>10</v>
@@ -1767,7 +1769,7 @@
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D11" s="20">
         <v>10</v>
@@ -1784,13 +1786,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D12" s="20">
         <v>10</v>
@@ -1807,13 +1809,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D13" s="20">
         <v>10</v>
@@ -1830,13 +1832,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D14" s="20">
         <v>10</v>
@@ -1853,13 +1855,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D15" s="20">
         <v>10</v>
@@ -1876,13 +1878,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D16" s="20">
         <v>10</v>
@@ -1899,13 +1901,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D17" s="20">
         <v>10</v>
@@ -1922,13 +1924,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D18" s="20">
         <v>10</v>
@@ -1945,13 +1947,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" s="20">
         <v>10</v>
@@ -1968,13 +1970,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D20" s="20">
         <v>10</v>
@@ -3218,7 +3220,7 @@
       <c r="G76">
         <v>75</v>
       </c>
-      <c r="H76" s="25" t="s">
+      <c r="H76" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3244,7 +3246,7 @@
       <c r="G77" s="15">
         <v>76</v>
       </c>
-      <c r="H77" s="26"/>
+      <c r="H77" s="28"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
@@ -3268,28 +3270,28 @@
       <c r="G78">
         <v>77</v>
       </c>
-      <c r="H78" s="26"/>
+      <c r="H78" s="28"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D79">
-        <v>10</v>
-      </c>
-      <c r="E79">
-        <v>2</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
+      <c r="D79" s="23">
+        <v>10</v>
+      </c>
+      <c r="E79" s="23">
+        <v>2</v>
+      </c>
+      <c r="F79" s="23">
+        <v>0</v>
+      </c>
+      <c r="G79" s="23">
         <v>78</v>
       </c>
     </row>
@@ -3301,7 +3303,7 @@
         <v>68</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80">
         <v>10</v>
@@ -5290,7 +5292,7 @@
         <v>141</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D174">
         <v>10</v>
@@ -5419,7 +5421,7 @@
         <v>143</v>
       </c>
       <c r="C180" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D180">
         <v>10</v>
@@ -5840,14 +5842,14 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B199" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C199" s="10" t="s">
-        <v>178</v>
+      <c r="C199" s="24" t="s">
+        <v>247</v>
       </c>
       <c r="D199">
         <v>10</v>
@@ -5884,7 +5886,7 @@
         <v>129</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D201">
         <v>10</v>
@@ -5907,7 +5909,7 @@
         <v>129</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D202" s="15">
         <v>10</v>
@@ -5930,7 +5932,7 @@
         <v>129</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D203">
         <v>10</v>
@@ -5953,7 +5955,7 @@
         <v>129</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D204">
         <v>10</v>
@@ -5990,7 +5992,7 @@
         <v>131</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D206">
         <v>10</v>
@@ -6013,7 +6015,7 @@
         <v>131</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D207" s="15">
         <v>10</v>
@@ -6036,7 +6038,7 @@
         <v>131</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D208">
         <v>10</v>
@@ -6059,7 +6061,7 @@
         <v>131</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D209">
         <v>10</v>
@@ -6078,11 +6080,11 @@
       <c r="A210" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B210" s="23" t="s">
+      <c r="B210" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C210" s="12" t="s">
         <v>187</v>
-      </c>
-      <c r="C210" s="12" t="s">
-        <v>188</v>
       </c>
       <c r="D210">
         <v>10</v>
@@ -6097,16 +6099,16 @@
         <v>209</v>
       </c>
       <c r="H210" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B211" s="24"/>
+      <c r="B211" s="26"/>
       <c r="C211" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D211" s="15">
         <v>10</v>
@@ -6125,11 +6127,11 @@
       <c r="A212" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B212" s="23" t="s">
-        <v>191</v>
+      <c r="B212" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="C212" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D212">
         <v>10</v>
@@ -6144,16 +6146,16 @@
         <v>211</v>
       </c>
       <c r="H212" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B213" s="24"/>
+      <c r="B213" s="26"/>
       <c r="C213" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D213" s="15">
         <v>10</v>
@@ -6172,11 +6174,11 @@
       <c r="A214" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B214" s="23" t="s">
-        <v>193</v>
+      <c r="B214" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D214">
         <v>10</v>
@@ -6191,16 +6193,16 @@
         <v>213</v>
       </c>
       <c r="H214" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B215" s="24"/>
+      <c r="B215" s="26"/>
       <c r="C215" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D215" s="15">
         <v>10</v>
@@ -6219,11 +6221,11 @@
       <c r="A216" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B216" s="23" t="s">
-        <v>195</v>
+      <c r="B216" s="25" t="s">
+        <v>194</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D216">
         <v>10</v>
@@ -6238,16 +6240,16 @@
         <v>215</v>
       </c>
       <c r="H216" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B217" s="24"/>
+      <c r="B217" s="26"/>
       <c r="C217" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D217" s="15">
         <v>10</v>
@@ -6266,11 +6268,11 @@
       <c r="A218" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B218" s="23" t="s">
-        <v>197</v>
+      <c r="B218" s="25" t="s">
+        <v>196</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D218">
         <v>10</v>
@@ -6285,16 +6287,16 @@
         <v>217</v>
       </c>
       <c r="H218" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B219" s="24"/>
+      <c r="B219" s="26"/>
       <c r="C219" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D219" s="15">
         <v>10</v>
@@ -6313,11 +6315,11 @@
       <c r="A220" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B220" s="23" t="s">
-        <v>199</v>
+      <c r="B220" s="25" t="s">
+        <v>198</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D220">
         <v>10</v>
@@ -6332,16 +6334,16 @@
         <v>219</v>
       </c>
       <c r="H220" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B221" s="24"/>
+      <c r="B221" s="26"/>
       <c r="C221" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D221" s="15">
         <v>10</v>
@@ -6360,11 +6362,11 @@
       <c r="A222" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B222" s="23" t="s">
-        <v>201</v>
+      <c r="B222" s="25" t="s">
+        <v>200</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D222">
         <v>10</v>
@@ -6379,16 +6381,16 @@
         <v>221</v>
       </c>
       <c r="H222" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B223" s="24"/>
+      <c r="B223" s="26"/>
       <c r="C223" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D223" s="15">
         <v>10</v>
@@ -6407,11 +6409,11 @@
       <c r="A224" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B224" s="23" t="s">
-        <v>203</v>
+      <c r="B224" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D224">
         <v>10</v>
@@ -6426,16 +6428,16 @@
         <v>223</v>
       </c>
       <c r="H224" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B225" s="24"/>
+      <c r="B225" s="26"/>
       <c r="C225" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D225" s="15">
         <v>10</v>
@@ -6466,11 +6468,11 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B227" s="3"/>
       <c r="C227" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D227" s="15">
         <v>10</v>
@@ -6487,11 +6489,11 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B228" s="3"/>
       <c r="C228" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D228" s="15">
         <v>10</v>
@@ -6508,11 +6510,11 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B229" s="3"/>
       <c r="C229" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D229" s="15">
         <v>10</v>
@@ -6546,7 +6548,7 @@
         <v>15</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3">
@@ -6567,7 +6569,7 @@
         <v>6</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C232" s="13"/>
       <c r="D232" s="13">
@@ -6588,7 +6590,7 @@
         <v>19</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="3">
@@ -6609,7 +6611,7 @@
         <v>153</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3">
@@ -6630,7 +6632,7 @@
         <v>66</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3">
@@ -6651,7 +6653,7 @@
         <v>11</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3">
@@ -6686,7 +6688,7 @@
         <v>15</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3">
@@ -6707,7 +6709,7 @@
         <v>6</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C239" s="13"/>
       <c r="D239" s="13">
@@ -6728,7 +6730,7 @@
         <v>19</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3">
@@ -6749,7 +6751,7 @@
         <v>153</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3">
@@ -6770,7 +6772,7 @@
         <v>66</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3">
@@ -6791,7 +6793,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3">
@@ -6812,7 +6814,7 @@
         <v>32</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3">
@@ -6830,7 +6832,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
@@ -6849,7 +6851,7 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
@@ -6868,7 +6870,7 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
@@ -6887,7 +6889,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
@@ -6906,7 +6908,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
@@ -6925,7 +6927,7 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
@@ -6944,7 +6946,7 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
@@ -7019,7 +7021,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>

</xml_diff>

<commit_message>
Updating the UEF macro to work on chambers 1-4 and fixing a bug on the bonus draw condition of FHR
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC0A55D-DF83-4090-A6E7-2EB8A69B84BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B90F70-0FAF-4D15-BD37-0353B2EE7D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PCs Only" sheetId="2" r:id="rId1"/>
+    <sheet name="All IP Addresses" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="292">
   <si>
     <t>Device</t>
   </si>
@@ -781,6 +782,138 @@
   </si>
   <si>
     <t>10.2.0.198</t>
+  </si>
+  <si>
+    <t>Lab Side IP</t>
+  </si>
+  <si>
+    <t>GEA Side IP</t>
+  </si>
+  <si>
+    <t>Server Computer</t>
+  </si>
+  <si>
+    <t>10.22.201.12</t>
+  </si>
+  <si>
+    <t>10.22.201.71</t>
+  </si>
+  <si>
+    <t>10.22.201.21</t>
+  </si>
+  <si>
+    <t>10.22.201.26</t>
+  </si>
+  <si>
+    <t>10.22.201.91</t>
+  </si>
+  <si>
+    <t>10.22.201.96</t>
+  </si>
+  <si>
+    <t>10.2.0.163</t>
+  </si>
+  <si>
+    <t>10.22.201.163</t>
+  </si>
+  <si>
+    <t>10.22.201.31</t>
+  </si>
+  <si>
+    <t>10.22.201.36</t>
+  </si>
+  <si>
+    <t>10.22.201.101</t>
+  </si>
+  <si>
+    <t>10.22.201.106</t>
+  </si>
+  <si>
+    <t>10.2.0.231</t>
+  </si>
+  <si>
+    <t>10.22.201.231</t>
+  </si>
+  <si>
+    <t>10.22.201.111</t>
+  </si>
+  <si>
+    <t>10.22.201.116</t>
+  </si>
+  <si>
+    <t>10.22.201.201</t>
+  </si>
+  <si>
+    <t>10.22.201.206</t>
+  </si>
+  <si>
+    <t>10.2.0.238</t>
+  </si>
+  <si>
+    <t>10.22.201.238</t>
+  </si>
+  <si>
+    <t>10.22.201.121</t>
+  </si>
+  <si>
+    <t>10.22.201.126</t>
+  </si>
+  <si>
+    <t>10.22.201.191</t>
+  </si>
+  <si>
+    <t>10.22.201.196</t>
+  </si>
+  <si>
+    <t>10.22.201.41</t>
+  </si>
+  <si>
+    <t>10.22.201.46</t>
+  </si>
+  <si>
+    <t>10.22.201.181</t>
+  </si>
+  <si>
+    <t>10.22.201.186</t>
+  </si>
+  <si>
+    <t>10.22.201.3</t>
+  </si>
+  <si>
+    <t>10.22.201.76</t>
+  </si>
+  <si>
+    <t>10.22.201.171</t>
+  </si>
+  <si>
+    <t>10.22.201.176</t>
+  </si>
+  <si>
+    <t>10.22.201.51</t>
+  </si>
+  <si>
+    <t>10.22.201.56</t>
+  </si>
+  <si>
+    <t>10.22.201.61</t>
+  </si>
+  <si>
+    <t>10.22.201.66</t>
+  </si>
+  <si>
+    <t>10.22.201.226</t>
+  </si>
+  <si>
+    <t>10.22.201.227</t>
+  </si>
+  <si>
+    <t>10.22.201.228</t>
+  </si>
+  <si>
+    <t>Temp Computer with FV LDO Software</t>
+  </si>
+  <si>
+    <t>10.2.0.8</t>
   </si>
 </sst>
 </file>
@@ -801,7 +934,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +956,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,13 +1064,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,6 +1104,125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B70B03-5E47-4C2F-B1EC-BDE939DBB1FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5735955" y="220980"/>
+          <a:ext cx="3223260" cy="2567940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>PC Login</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.\99700001z</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WIN_10l0cal</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>All PCs use the same username and password</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>For Remote Desktop Connection the 10.22.201.XXX IP should be used</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>You must be logged</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> into "GlobalProtect" VPN</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1394,211 +1658,935 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39906FB2-DCE1-4053-B4B2-D81A453EB460}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="252" max="252" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="508" max="508" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="510" max="510" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="764" max="764" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="766" max="766" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1020" max="1020" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1022" max="1022" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1276" max="1276" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1278" max="1278" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1532" max="1532" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1534" max="1534" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1788" max="1788" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1790" max="1790" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2044" max="2044" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2046" max="2046" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2300" max="2300" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2302" max="2302" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2556" max="2556" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2558" max="2558" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2812" max="2812" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2814" max="2814" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3068" max="3068" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3070" max="3070" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3324" max="3324" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3326" max="3326" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3580" max="3580" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3582" max="3582" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3836" max="3836" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3838" max="3838" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4092" max="4092" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4094" max="4094" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4348" max="4348" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4350" max="4350" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4604" max="4604" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4606" max="4606" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4860" max="4860" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4862" max="4862" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5116" max="5116" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5118" max="5118" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5372" max="5372" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5374" max="5374" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5628" max="5628" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5630" max="5630" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5884" max="5884" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5886" max="5886" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6140" max="6140" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6142" max="6142" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6396" max="6396" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6398" max="6398" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6652" max="6652" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6654" max="6654" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6908" max="6908" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6910" max="6910" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7164" max="7164" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7166" max="7166" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7420" max="7420" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7422" max="7422" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7676" max="7676" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7678" max="7678" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7932" max="7932" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7934" max="7934" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8188" max="8188" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8190" max="8190" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8444" max="8444" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8446" max="8446" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8700" max="8700" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8702" max="8702" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8956" max="8956" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8958" max="8958" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9212" max="9212" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9214" max="9214" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9468" max="9468" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9470" max="9470" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9724" max="9724" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9726" max="9726" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9980" max="9980" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9982" max="9982" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10236" max="10236" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10238" max="10238" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10492" max="10492" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10494" max="10494" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10748" max="10748" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10750" max="10750" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11004" max="11004" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11006" max="11006" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11260" max="11260" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11262" max="11262" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11516" max="11516" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11518" max="11518" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11772" max="11772" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11774" max="11774" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12028" max="12028" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12030" max="12030" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12284" max="12284" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12286" max="12286" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12540" max="12540" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12542" max="12542" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12796" max="12796" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12798" max="12798" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13052" max="13052" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13054" max="13054" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13308" max="13308" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13310" max="13310" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13564" max="13564" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13566" max="13566" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13820" max="13820" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13822" max="13822" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14076" max="14076" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14078" max="14078" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14332" max="14332" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14334" max="14334" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14588" max="14588" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14590" max="14590" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14844" max="14844" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14846" max="14846" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15100" max="15100" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15102" max="15102" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15356" max="15356" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15358" max="15358" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15612" max="15612" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15614" max="15614" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15868" max="15868" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15870" max="15870" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16124" max="16124" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="16126" max="16126" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="str">
+        <f>'[1]Asset Numbers'!B17</f>
+        <v>Hybrid Electric Water Heater Test Station</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="24" t="str">
+        <f>'[1]Asset Numbers'!E17</f>
+        <v>10.2.0.21</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="str">
+        <f>'[1]Asset Numbers'!B22</f>
+        <v>Hybrid Electric Water Heater Test Station</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="24" t="str">
+        <f>'[1]Asset Numbers'!E22</f>
+        <v>10.2.0.26</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="str">
+        <f>'[1]Asset Numbers'!B27</f>
+        <v>Hybrid Electric Water Heater Test Station</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="24" t="str">
+        <f>'[1]Asset Numbers'!E27</f>
+        <v>10.2.0.91</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6BCF3-52DA-45D5-A06F-31378179F4D8}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="L86" sqref="L86"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="771" max="771" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="1027" max="1027" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="1283" max="1283" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="1539" max="1539" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="1795" max="1795" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2051" max="2051" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2307" max="2307" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2563" max="2563" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2819" max="2819" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3075" max="3075" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3331" max="3331" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3587" max="3587" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3843" max="3843" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4099" max="4099" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4355" max="4355" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4611" max="4611" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4867" max="4867" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5123" max="5123" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5379" max="5379" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5635" max="5635" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5891" max="5891" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6147" max="6147" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6403" max="6403" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6659" max="6659" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6915" max="6915" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="7171" max="7171" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="7427" max="7427" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="7683" max="7683" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="7939" max="7939" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="8195" max="8195" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="8451" max="8451" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="8707" max="8707" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="8963" max="8963" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="9219" max="9219" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="9475" max="9475" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="9731" max="9731" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="9987" max="9987" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="10243" max="10243" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="10499" max="10499" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="10755" max="10755" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11011" max="11011" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11267" max="11267" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11523" max="11523" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="11779" max="11779" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="12035" max="12035" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="12291" max="12291" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="12547" max="12547" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="12803" max="12803" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="13059" max="13059" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="13315" max="13315" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="13571" max="13571" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="13827" max="13827" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="14083" max="14083" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="14339" max="14339" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="14595" max="14595" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="14851" max="14851" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="15107" max="15107" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="15363" max="15363" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="15619" max="15619" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="15875" max="15875" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="16131" max="16131" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1619,7 +2607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>10</v>
       </c>
@@ -1633,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>10</v>
       </c>
@@ -1647,7 +2635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +2658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>10</v>
       </c>
@@ -1684,7 +2672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>10</v>
       </c>
@@ -1698,7 +2686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>10</v>
       </c>
@@ -1712,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>10</v>
       </c>
@@ -1726,7 +2714,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" t="s">
+        <v>291</v>
+      </c>
       <c r="D9">
         <v>10</v>
       </c>
@@ -1740,292 +2737,292 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="3" t="s">
         <v>246</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D10" s="20">
-        <v>10</v>
-      </c>
-      <c r="E10" s="20">
-        <v>2</v>
-      </c>
-      <c r="F10" s="20">
-        <v>0</v>
-      </c>
-      <c r="G10" s="20">
+      <c r="D10" s="3">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="20">
-        <v>10</v>
-      </c>
-      <c r="E11" s="20">
-        <v>2</v>
-      </c>
-      <c r="F11" s="20">
-        <v>0</v>
-      </c>
-      <c r="G11" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="3" t="s">
         <v>246</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D12" s="20">
-        <v>10</v>
-      </c>
-      <c r="E12" s="20">
-        <v>2</v>
-      </c>
-      <c r="F12" s="20">
-        <v>0</v>
-      </c>
-      <c r="G12" s="20">
+      <c r="D12" s="3">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="20">
-        <v>10</v>
-      </c>
-      <c r="E13" s="20">
-        <v>2</v>
-      </c>
-      <c r="F13" s="20">
-        <v>0</v>
-      </c>
-      <c r="G13" s="20">
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="3" t="s">
         <v>244</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D14" s="20">
-        <v>10</v>
-      </c>
-      <c r="E14" s="20">
-        <v>2</v>
-      </c>
-      <c r="F14" s="20">
-        <v>0</v>
-      </c>
-      <c r="G14" s="20">
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D15" s="20">
-        <v>10</v>
-      </c>
-      <c r="E15" s="20">
-        <v>2</v>
-      </c>
-      <c r="F15" s="20">
-        <v>0</v>
-      </c>
-      <c r="G15" s="20">
+      <c r="D15" s="3">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D16" s="20">
-        <v>10</v>
-      </c>
-      <c r="E16" s="20">
-        <v>2</v>
-      </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
-      <c r="G16" s="20">
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="20">
-        <v>10</v>
-      </c>
-      <c r="E17" s="20">
-        <v>2</v>
-      </c>
-      <c r="F17" s="20">
-        <v>0</v>
-      </c>
-      <c r="G17" s="20">
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D18" s="20">
-        <v>10</v>
-      </c>
-      <c r="E18" s="20">
-        <v>2</v>
-      </c>
-      <c r="F18" s="20">
-        <v>0</v>
-      </c>
-      <c r="G18" s="20">
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="3" t="s">
         <v>244</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D19" s="20">
-        <v>10</v>
-      </c>
-      <c r="E19" s="20">
-        <v>2</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0</v>
-      </c>
-      <c r="G19" s="20">
+      <c r="D19" s="3">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D20" s="20">
-        <v>10</v>
-      </c>
-      <c r="E20" s="20">
-        <v>2</v>
-      </c>
-      <c r="F20" s="20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="20">
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="str">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="str">
         <f>'[1]Asset Numbers'!B16</f>
         <v>Data Aquisition System Yokogawa MW100 w IO Cards</v>
       </c>
-      <c r="B21" s="20" t="str">
+      <c r="B21" s="3" t="str">
         <f>'[1]Asset Numbers'!D16</f>
         <v>1A</v>
       </c>
-      <c r="C21" s="20" t="str">
+      <c r="C21" s="3" t="str">
         <f>'[1]Asset Numbers'!E16</f>
         <v>10.2.0.20</v>
       </c>
-      <c r="D21" s="20">
-        <v>10</v>
-      </c>
-      <c r="E21" s="20">
-        <v>2</v>
-      </c>
-      <c r="F21" s="20">
-        <v>0</v>
-      </c>
-      <c r="G21" s="20">
+      <c r="D21" s="3">
+        <v>10</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="str">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="str">
         <f>'[1]Asset Numbers'!B17</f>
         <v>Hybrid Electric Water Heater Test Station</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="21" t="str">
+      <c r="B22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18" t="str">
         <f>'[1]Asset Numbers'!E17</f>
         <v>10.2.0.21</v>
       </c>
@@ -2042,7 +3039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f>'[1]Asset Numbers'!B20</f>
         <v>Agilent 34972A Data Logger</v>
@@ -2067,7 +3064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +3087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>10</v>
       </c>
@@ -2104,7 +3101,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f>'[1]Asset Numbers'!B21</f>
         <v>Data Aquisition System Yokogawa MW100 w IO Cards</v>
@@ -2130,7 +3127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="str">
         <f>'[1]Asset Numbers'!B22</f>
         <v>Hybrid Electric Water Heater Test Station</v>
@@ -2155,7 +3152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f>'[1]Asset Numbers'!B25</f>
         <v>Agilent 34972A Data Logger</v>
@@ -2180,7 +3177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2203,7 +3200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>10</v>
       </c>
@@ -2217,7 +3214,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -2240,7 +3237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>6</v>
       </c>
@@ -2263,7 +3260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
@@ -2286,7 +3283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>11</v>
       </c>
@@ -2309,7 +3306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>10</v>
       </c>
@@ -2323,7 +3320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
@@ -2346,7 +3343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>6</v>
       </c>
@@ -2369,7 +3366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
@@ -2392,7 +3389,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>11</v>
       </c>
@@ -2415,7 +3412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>10</v>
       </c>
@@ -2429,7 +3426,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
@@ -2452,7 +3449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>6</v>
       </c>
@@ -2475,7 +3472,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
@@ -2498,7 +3495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +3518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>32</v>
       </c>
@@ -2544,7 +3541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
@@ -2567,7 +3564,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>6</v>
       </c>
@@ -2590,7 +3587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>19</v>
       </c>
@@ -2613,7 +3610,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>11</v>
       </c>
@@ -2636,7 +3633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>32</v>
       </c>
@@ -2659,7 +3656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -2682,7 +3679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +3702,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>19</v>
       </c>
@@ -2728,7 +3725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>11</v>
       </c>
@@ -2751,7 +3748,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>10</v>
       </c>
@@ -2765,7 +3762,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>15</v>
       </c>
@@ -2788,7 +3785,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>6</v>
       </c>
@@ -2811,7 +3808,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
@@ -2834,7 +3831,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D59">
         <v>10</v>
       </c>
@@ -2848,7 +3845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>10</v>
       </c>
@@ -2862,7 +3859,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
@@ -2885,7 +3882,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>6</v>
       </c>
@@ -2908,7 +3905,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>19</v>
       </c>
@@ -2931,7 +3928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>11</v>
       </c>
@@ -2954,7 +3951,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>10</v>
       </c>
@@ -2968,7 +3965,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>15</v>
       </c>
@@ -2991,7 +3988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>6</v>
       </c>
@@ -3014,7 +4011,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>19</v>
       </c>
@@ -3037,7 +4034,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>11</v>
       </c>
@@ -3060,7 +4057,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -3083,7 +4080,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>15</v>
       </c>
@@ -3106,7 +4103,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>6</v>
       </c>
@@ -3129,7 +4126,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>19</v>
       </c>
@@ -3152,7 +4149,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>64</v>
       </c>
@@ -3175,7 +4172,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -3198,7 +4195,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>15</v>
       </c>
@@ -3224,7 +4221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>6</v>
       </c>
@@ -3248,7 +4245,7 @@
       </c>
       <c r="H77" s="28"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>19</v>
       </c>
@@ -3272,7 +4269,7 @@
       </c>
       <c r="H78" s="28"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>11</v>
       </c>
@@ -3282,27 +4279,27 @@
       <c r="C79" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D79" s="23">
-        <v>10</v>
-      </c>
-      <c r="E79" s="23">
-        <v>2</v>
-      </c>
-      <c r="F79" s="23">
-        <v>0</v>
-      </c>
-      <c r="G79" s="23">
+      <c r="D79" s="20">
+        <v>10</v>
+      </c>
+      <c r="E79" s="20">
+        <v>2</v>
+      </c>
+      <c r="F79" s="20">
+        <v>0</v>
+      </c>
+      <c r="G79" s="20">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B80" s="19" t="s">
+      <c r="B80" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="3" t="s">
         <v>214</v>
       </c>
       <c r="D80">
@@ -3318,7 +4315,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>15</v>
       </c>
@@ -3341,7 +4338,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>75</v>
       </c>
@@ -3358,7 +4355,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>19</v>
       </c>
@@ -3381,7 +4378,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>11</v>
       </c>
@@ -3404,14 +4401,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D85">
@@ -3427,7 +4424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D86">
         <v>10</v>
       </c>
@@ -3441,7 +4438,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D87">
         <v>10</v>
       </c>
@@ -3455,7 +4452,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D88">
         <v>10</v>
       </c>
@@ -3469,7 +4466,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D89">
         <v>10</v>
       </c>
@@ -3483,7 +4480,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D90">
         <v>10</v>
       </c>
@@ -3497,7 +4494,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="str">
         <f>'[1]Asset Numbers'!B26</f>
         <v>Data Aquisition System Yokogawa MW100 w IO Cards</v>
@@ -3523,7 +4520,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="str">
         <f>'[1]Asset Numbers'!B27</f>
         <v>Hybrid Electric Water Heater Test Station</v>
@@ -3548,7 +4545,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="str">
         <f>'[1]Asset Numbers'!B30</f>
         <v>Agilent 34972A Data Logger</v>
@@ -3573,7 +4570,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>11</v>
       </c>
@@ -3596,7 +4593,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D95">
         <v>10</v>
       </c>
@@ -3610,7 +4607,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>15</v>
       </c>
@@ -3633,7 +4630,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>6</v>
       </c>
@@ -3656,7 +4653,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>19</v>
       </c>
@@ -3679,7 +4676,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>11</v>
       </c>
@@ -3702,7 +4699,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D100">
         <v>10</v>
       </c>
@@ -3716,7 +4713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>15</v>
       </c>
@@ -3739,7 +4736,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>6</v>
       </c>
@@ -3762,7 +4759,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>19</v>
       </c>
@@ -3785,7 +4782,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>11</v>
       </c>
@@ -3808,7 +4805,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D105">
         <v>10</v>
       </c>
@@ -3822,7 +4819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>15</v>
       </c>
@@ -3845,7 +4842,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>6</v>
       </c>
@@ -3868,7 +4865,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>19</v>
       </c>
@@ -3891,7 +4888,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>11</v>
       </c>
@@ -3914,7 +4911,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D110">
         <v>10</v>
       </c>
@@ -3928,7 +4925,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>15</v>
       </c>
@@ -3951,7 +4948,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>6</v>
       </c>
@@ -3974,7 +4971,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>19</v>
       </c>
@@ -3997,7 +4994,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>11</v>
       </c>
@@ -4020,7 +5017,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D115">
         <v>10</v>
       </c>
@@ -4034,7 +5031,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>15</v>
       </c>
@@ -4057,7 +5054,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>6</v>
       </c>
@@ -4080,7 +5077,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>19</v>
       </c>
@@ -4103,7 +5100,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>11</v>
       </c>
@@ -4126,7 +5123,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D120">
         <v>10</v>
       </c>
@@ -4140,7 +5137,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>15</v>
       </c>
@@ -4163,7 +5160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>6</v>
       </c>
@@ -4186,7 +5183,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>19</v>
       </c>
@@ -4209,7 +5206,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>11</v>
       </c>
@@ -4232,7 +5229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D125">
         <v>10</v>
       </c>
@@ -4246,7 +5243,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>15</v>
       </c>
@@ -4269,7 +5266,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
         <v>6</v>
       </c>
@@ -4292,7 +5289,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>19</v>
       </c>
@@ -4315,7 +5312,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>11</v>
       </c>
@@ -4338,7 +5335,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D130">
         <v>10</v>
       </c>
@@ -4352,7 +5349,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>115</v>
       </c>
@@ -4375,7 +5372,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>115</v>
       </c>
@@ -4398,7 +5395,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>115</v>
       </c>
@@ -4421,7 +5418,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>115</v>
       </c>
@@ -4444,7 +5441,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="str">
         <f>'[1]Asset Numbers'!B18</f>
         <v>WT310 Power Analyzer</v>
@@ -4469,7 +5466,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="str">
         <f>'[1]Asset Numbers'!B23</f>
         <v>WT310 Power Analyzer</v>
@@ -4494,7 +5491,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="str">
         <f>'[1]Asset Numbers'!B28</f>
         <v>WT310 Power Analyzer</v>
@@ -4519,7 +5516,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>115</v>
       </c>
@@ -4542,7 +5539,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>115</v>
       </c>
@@ -4565,7 +5562,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>115</v>
       </c>
@@ -4588,7 +5585,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>115</v>
       </c>
@@ -4611,7 +5608,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>115</v>
       </c>
@@ -4634,7 +5631,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>115</v>
       </c>
@@ -4657,7 +5654,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>115</v>
       </c>
@@ -4680,7 +5677,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>115</v>
       </c>
@@ -4703,7 +5700,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>115</v>
       </c>
@@ -4726,7 +5723,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>115</v>
       </c>
@@ -4749,7 +5746,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>115</v>
       </c>
@@ -4772,7 +5769,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>115</v>
       </c>
@@ -4795,7 +5792,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>115</v>
       </c>
@@ -4818,7 +5815,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>115</v>
       </c>
@@ -4841,7 +5838,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>115</v>
       </c>
@@ -4864,7 +5861,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>115</v>
       </c>
@@ -4887,7 +5884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>115</v>
       </c>
@@ -4910,7 +5907,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D155">
         <v>10</v>
       </c>
@@ -4924,7 +5921,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>145</v>
       </c>
@@ -4945,7 +5942,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>146</v>
       </c>
@@ -4968,7 +5965,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>148</v>
       </c>
@@ -4989,7 +5986,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>149</v>
       </c>
@@ -5010,7 +6007,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D160">
         <v>10</v>
       </c>
@@ -5024,7 +6021,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>150</v>
       </c>
@@ -5047,7 +6044,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D162">
         <v>10</v>
       </c>
@@ -5061,7 +6058,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>15</v>
       </c>
@@ -5082,7 +6079,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>6</v>
       </c>
@@ -5103,7 +6100,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>19</v>
       </c>
@@ -5124,7 +6121,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>153</v>
       </c>
@@ -5145,7 +6142,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>66</v>
       </c>
@@ -5166,7 +6163,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>11</v>
       </c>
@@ -5187,7 +6184,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D169">
         <v>10</v>
       </c>
@@ -5201,7 +6198,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D170">
         <v>10</v>
       </c>
@@ -5215,7 +6212,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>15</v>
       </c>
@@ -5238,7 +6235,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>6</v>
       </c>
@@ -5261,7 +6258,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>19</v>
       </c>
@@ -5284,7 +6281,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>32</v>
       </c>
@@ -5307,7 +6304,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D175">
         <v>10</v>
       </c>
@@ -5321,7 +6318,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>15</v>
       </c>
@@ -5344,7 +6341,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
         <v>6</v>
       </c>
@@ -5367,7 +6364,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>19</v>
       </c>
@@ -5390,7 +6387,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>11</v>
       </c>
@@ -5413,14 +6410,14 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B180" s="18" t="s">
+      <c r="B180" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C180" s="18" t="s">
+      <c r="C180" s="5" t="s">
         <v>216</v>
       </c>
       <c r="D180">
@@ -5436,7 +6433,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>15</v>
       </c>
@@ -5459,7 +6456,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
         <v>6</v>
       </c>
@@ -5482,7 +6479,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>19</v>
       </c>
@@ -5505,7 +6502,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>11</v>
       </c>
@@ -5528,7 +6525,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>32</v>
       </c>
@@ -5551,7 +6548,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>15</v>
       </c>
@@ -5574,7 +6571,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="13" t="s">
         <v>6</v>
       </c>
@@ -5597,7 +6594,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>19</v>
       </c>
@@ -5620,7 +6617,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>11</v>
       </c>
@@ -5643,7 +6640,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>32</v>
       </c>
@@ -5666,7 +6663,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>15</v>
       </c>
@@ -5689,7 +6686,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
         <v>6</v>
       </c>
@@ -5712,7 +6709,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>19</v>
       </c>
@@ -5735,7 +6732,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>11</v>
       </c>
@@ -5758,7 +6755,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D195">
         <v>10</v>
       </c>
@@ -5772,7 +6769,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>15</v>
       </c>
@@ -5795,7 +6792,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
         <v>6</v>
       </c>
@@ -5818,7 +6815,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>19</v>
       </c>
@@ -5841,14 +6838,14 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B199" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C199" s="24" t="s">
+      <c r="C199" s="21" t="s">
         <v>247</v>
       </c>
       <c r="D199">
@@ -5864,7 +6861,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D200">
         <v>10</v>
       </c>
@@ -5878,7 +6875,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>15</v>
       </c>
@@ -5901,7 +6898,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
         <v>6</v>
       </c>
@@ -5924,7 +6921,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>19</v>
       </c>
@@ -5947,7 +6944,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>11</v>
       </c>
@@ -5970,7 +6967,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D205">
         <v>10</v>
       </c>
@@ -5984,7 +6981,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>15</v>
       </c>
@@ -6007,7 +7004,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="14" t="s">
         <v>6</v>
       </c>
@@ -6030,7 +7027,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>19</v>
       </c>
@@ -6053,7 +7050,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>11</v>
       </c>
@@ -6076,7 +7073,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
         <v>15</v>
       </c>
@@ -6102,7 +7099,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>6</v>
       </c>
@@ -6123,7 +7120,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
         <v>15</v>
       </c>
@@ -6149,7 +7146,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>6</v>
       </c>
@@ -6170,7 +7167,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
         <v>15</v>
       </c>
@@ -6196,7 +7193,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>6</v>
       </c>
@@ -6217,7 +7214,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
         <v>15</v>
       </c>
@@ -6243,7 +7240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>6</v>
       </c>
@@ -6264,7 +7261,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
         <v>15</v>
       </c>
@@ -6290,7 +7287,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>6</v>
       </c>
@@ -6311,7 +7308,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>15</v>
       </c>
@@ -6337,7 +7334,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>6</v>
       </c>
@@ -6358,7 +7355,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
         <v>15</v>
       </c>
@@ -6384,7 +7381,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>6</v>
       </c>
@@ -6405,7 +7402,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>15</v>
       </c>
@@ -6431,7 +7428,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>6</v>
       </c>
@@ -6452,7 +7449,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D226">
         <v>10</v>
       </c>
@@ -6466,7 +7463,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>204</v>
       </c>
@@ -6487,7 +7484,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>206</v>
       </c>
@@ -6508,7 +7505,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>208</v>
       </c>
@@ -6529,7 +7526,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D230">
         <v>10</v>
       </c>
@@ -6543,7 +7540,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>15</v>
       </c>
@@ -6564,7 +7561,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
         <v>6</v>
       </c>
@@ -6585,7 +7582,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>19</v>
       </c>
@@ -6606,7 +7603,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>153</v>
       </c>
@@ -6627,7 +7624,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>66</v>
       </c>
@@ -6648,7 +7645,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>11</v>
       </c>
@@ -6669,7 +7666,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D237">
         <v>10</v>
       </c>
@@ -6683,7 +7680,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>15</v>
       </c>
@@ -6704,7 +7701,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="13" t="s">
         <v>6</v>
       </c>
@@ -6725,7 +7722,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>19</v>
       </c>
@@ -6746,7 +7743,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>153</v>
       </c>
@@ -6767,7 +7764,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>66</v>
       </c>
@@ -6788,7 +7785,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>11</v>
       </c>
@@ -6809,7 +7806,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>32</v>
       </c>
@@ -6830,8 +7827,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A245" s="20" t="s">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B245" s="3"/>
@@ -6849,8 +7846,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A246" s="20" t="s">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
         <v>218</v>
       </c>
       <c r="B246" s="3"/>
@@ -6868,8 +7865,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A247" s="20" t="s">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
         <v>219</v>
       </c>
       <c r="B247" s="3"/>
@@ -6887,8 +7884,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A248" s="20" t="s">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
         <v>220</v>
       </c>
       <c r="B248" s="3"/>
@@ -6906,8 +7903,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A249" s="20" t="s">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B249" s="3"/>
@@ -6925,8 +7922,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A250" s="20" t="s">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
         <v>222</v>
       </c>
       <c r="B250" s="3"/>
@@ -6944,8 +7941,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A251" s="20" t="s">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
         <v>223</v>
       </c>
       <c r="B251" s="3"/>
@@ -6963,7 +7960,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D252">
         <v>10</v>
       </c>
@@ -6977,7 +7974,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D253">
         <v>10</v>
       </c>
@@ -6991,7 +7988,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D254">
         <v>10</v>
       </c>
@@ -7005,7 +8002,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D255">
         <v>10</v>
       </c>
@@ -7019,7 +8016,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
Improving lab throughput for UEF testing
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC255760-0DA1-4AA9-B2A8-E1E3B215AF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCB67D7-CC9E-466E-B3A7-2BF5FB99602B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
   </bookViews>
@@ -730,9 +730,6 @@
     <t>Allen Bradley Compact Logic 5380</t>
   </si>
   <si>
-    <t>Computer PC with LabView/Studio 5000</t>
-  </si>
-  <si>
     <t xml:space="preserve">FV ICPCON 7188E8 RS232 Gateway	</t>
   </si>
   <si>
@@ -944,6 +941,9 @@
   </si>
   <si>
     <t>10.22.201.86</t>
+  </si>
+  <si>
+    <t>Computer PC with Studio 5000</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1125,6 +1125,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1136,16 +1145,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1421,9 +1420,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1461,7 +1460,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1567,7 +1566,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1709,7 +1708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1925,22 +1924,22 @@
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>248</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,7 +1953,7 @@
         <v>62</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,7 +1969,7 @@
         <v>10.2.0.21</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +1985,7 @@
         <v>10.2.0.26</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,7 +2001,7 @@
         <v>10.2.0.91</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2016,7 +2015,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2027,10 +2026,10 @@
         <v>152</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>257</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,7 +2043,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2057,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,7 +2071,7 @@
         <v>87</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2086,7 +2085,7 @@
         <v>92</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,10 +2096,10 @@
         <v>210</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>263</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,7 +2113,7 @@
         <v>97</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2127,7 @@
         <v>102</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2141,7 @@
         <v>179</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2156,7 +2155,7 @@
         <v>183</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,10 +2166,10 @@
         <v>211</v>
       </c>
       <c r="C18" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>269</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,7 +2183,7 @@
         <v>107</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,7 +2197,7 @@
         <v>112</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,7 +2211,7 @@
         <v>172</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,7 +2225,7 @@
         <v>176</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,7 +2239,7 @@
         <v>29</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,7 +2253,7 @@
         <v>36</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,7 +2267,7 @@
         <v>162</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,7 +2281,7 @@
         <v>167</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,7 +2295,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,7 +2309,7 @@
         <v>71</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,7 +2323,7 @@
         <v>155</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,7 +2337,7 @@
         <v>158</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,7 +2351,7 @@
         <v>42</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,7 +2365,7 @@
         <v>47</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,7 +2379,7 @@
         <v>51</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,7 +2393,7 @@
         <v>56</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2406,7 +2405,7 @@
         <v>205</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2418,7 +2417,7 @@
         <v>207</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2430,35 +2429,35 @@
         <v>209</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>296</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="C39" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="D39" s="30" t="s">
         <v>300</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2471,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6BCF3-52DA-45D5-A06F-31378179F4D8}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2692,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2797,10 +2796,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -2818,13 +2817,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
         <v>290</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C9" t="s">
-        <v>291</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2842,13 +2841,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>230</v>
+        <v>301</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
@@ -2870,7 +2869,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -2891,10 +2890,10 @@
         <v>229</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -2912,13 +2911,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -2936,13 +2935,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D14" s="3">
         <v>10</v>
@@ -2963,10 +2962,10 @@
         <v>225</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D15" s="3">
         <v>10</v>
@@ -2987,10 +2986,10 @@
         <v>224</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D16" s="3">
         <v>10</v>
@@ -3011,10 +3010,10 @@
         <v>226</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -3035,10 +3034,10 @@
         <v>227</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
@@ -3059,10 +3058,10 @@
         <v>226</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D19" s="3">
         <v>10</v>
@@ -3083,10 +3082,10 @@
         <v>228</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D20" s="3">
         <v>10</v>
@@ -3799,7 +3798,7 @@
         <v>49</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4388,7 +4387,7 @@
       <c r="G76">
         <v>75</v>
       </c>
-      <c r="H76" s="30" t="s">
+      <c r="H76" s="33" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4414,7 +4413,7 @@
       <c r="G77" s="15">
         <v>76</v>
       </c>
-      <c r="H77" s="31"/>
+      <c r="H77" s="34"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -4438,7 +4437,7 @@
       <c r="G78">
         <v>77</v>
       </c>
-      <c r="H78" s="31"/>
+      <c r="H78" s="34"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
@@ -4615,17 +4614,17 @@
       <c r="G86">
         <v>85</v>
       </c>
-      <c r="H86" s="32"/>
+      <c r="H86" s="28"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B87" s="34" t="s">
+      <c r="C87" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="C87" s="34" t="s">
-        <v>300</v>
       </c>
       <c r="D87" s="3">
         <v>10</v>
@@ -4654,7 +4653,7 @@
       <c r="G88">
         <v>87</v>
       </c>
-      <c r="H88" s="33"/>
+      <c r="H88" s="29"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D89">
@@ -7146,7 +7145,7 @@
         <v>137</v>
       </c>
       <c r="C199" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D199">
         <v>10</v>
@@ -7388,7 +7387,7 @@
       <c r="A210" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B210" s="28" t="s">
+      <c r="B210" s="31" t="s">
         <v>186</v>
       </c>
       <c r="C210" s="12" t="s">
@@ -7414,7 +7413,7 @@
       <c r="A211" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B211" s="29"/>
+      <c r="B211" s="32"/>
       <c r="C211" s="14" t="s">
         <v>189</v>
       </c>
@@ -7436,7 +7435,7 @@
       <c r="A212" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B212" s="28" t="s">
+      <c r="B212" s="31" t="s">
         <v>190</v>
       </c>
       <c r="C212" s="12" t="s">
@@ -7462,7 +7461,7 @@
       <c r="A213" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B213" s="29"/>
+      <c r="B213" s="32"/>
       <c r="C213" s="14" t="s">
         <v>191</v>
       </c>
@@ -7484,7 +7483,7 @@
       <c r="A214" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B214" s="28" t="s">
+      <c r="B214" s="31" t="s">
         <v>192</v>
       </c>
       <c r="C214" s="12" t="s">
@@ -7510,7 +7509,7 @@
       <c r="A215" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B215" s="29"/>
+      <c r="B215" s="32"/>
       <c r="C215" s="14" t="s">
         <v>193</v>
       </c>
@@ -7532,7 +7531,7 @@
       <c r="A216" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B216" s="28" t="s">
+      <c r="B216" s="31" t="s">
         <v>194</v>
       </c>
       <c r="C216" s="12" t="s">
@@ -7558,7 +7557,7 @@
       <c r="A217" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B217" s="29"/>
+      <c r="B217" s="32"/>
       <c r="C217" s="14" t="s">
         <v>195</v>
       </c>
@@ -7580,7 +7579,7 @@
       <c r="A218" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B218" s="28" t="s">
+      <c r="B218" s="31" t="s">
         <v>196</v>
       </c>
       <c r="C218" s="12" t="s">
@@ -7606,7 +7605,7 @@
       <c r="A219" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B219" s="29"/>
+      <c r="B219" s="32"/>
       <c r="C219" s="14" t="s">
         <v>197</v>
       </c>
@@ -7628,7 +7627,7 @@
       <c r="A220" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B220" s="28" t="s">
+      <c r="B220" s="31" t="s">
         <v>198</v>
       </c>
       <c r="C220" s="12" t="s">
@@ -7654,7 +7653,7 @@
       <c r="A221" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B221" s="29"/>
+      <c r="B221" s="32"/>
       <c r="C221" s="14" t="s">
         <v>199</v>
       </c>
@@ -7676,7 +7675,7 @@
       <c r="A222" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B222" s="28" t="s">
+      <c r="B222" s="31" t="s">
         <v>200</v>
       </c>
       <c r="C222" s="12" t="s">
@@ -7702,7 +7701,7 @@
       <c r="A223" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B223" s="29"/>
+      <c r="B223" s="32"/>
       <c r="C223" s="14" t="s">
         <v>201</v>
       </c>
@@ -7724,7 +7723,7 @@
       <c r="A224" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B224" s="28" t="s">
+      <c r="B224" s="31" t="s">
         <v>202</v>
       </c>
       <c r="C224" s="12" t="s">
@@ -7750,7 +7749,7 @@
       <c r="A225" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B225" s="29"/>
+      <c r="B225" s="32"/>
       <c r="C225" s="14" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Making architecture changes to simply code
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Documentation/IP Addresses Water Lab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCB67D7-CC9E-466E-B3A7-2BF5FB99602B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FE8D39-320E-410F-9B50-19F85BF7BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{516DDD93-702F-4F3F-A190-A14C63473A95}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="305">
   <si>
     <t>Device</t>
   </si>
@@ -490,12 +490,6 @@
     <t>Gas Meter 6D</t>
   </si>
   <si>
-    <t>Chamber 5 Temperature/Humidity Sensor</t>
-  </si>
-  <si>
-    <t>10.2.0.160</t>
-  </si>
-  <si>
     <t>2 ED</t>
   </si>
   <si>
@@ -944,6 +938,21 @@
   </si>
   <si>
     <t>Computer PC with Studio 5000</t>
+  </si>
+  <si>
+    <t>Viasala Temp and RH 5A and 5B</t>
+  </si>
+  <si>
+    <t>10.2.0.39</t>
+  </si>
+  <si>
+    <t>Chamber 5 Temperature/Humidity Sensor Indigo</t>
+  </si>
+  <si>
+    <t>5A and 5C</t>
+  </si>
+  <si>
+    <t>10.2.0.161</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1134,6 +1143,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1924,22 +1935,22 @@
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,7 +1964,7 @@
         <v>62</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +1980,7 @@
         <v>10.2.0.21</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1996,7 @@
         <v>10.2.0.26</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2001,7 +2012,7 @@
         <v>10.2.0.91</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2015,7 +2026,7 @@
         <v>82</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,13 +2034,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,7 +2054,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,7 +2068,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2071,7 +2082,7 @@
         <v>87</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2085,7 +2096,7 @@
         <v>92</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,13 +2104,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2113,7 +2124,7 @@
         <v>97</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,7 +2138,7 @@
         <v>102</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,10 +2149,10 @@
         <v>129</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,10 +2163,10 @@
         <v>131</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2163,13 +2174,13 @@
         <v>6</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2194,7 @@
         <v>107</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2208,7 @@
         <v>112</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2208,10 +2219,10 @@
         <v>135</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,10 +2233,10 @@
         <v>137</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,7 +2250,7 @@
         <v>29</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2253,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2264,10 +2275,10 @@
         <v>118</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2278,10 +2289,10 @@
         <v>120</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2295,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2309,7 +2320,7 @@
         <v>71</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2320,10 +2331,10 @@
         <v>141</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2334,10 +2345,10 @@
         <v>143</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2351,7 +2362,7 @@
         <v>42</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2365,7 +2376,7 @@
         <v>47</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2379,7 +2390,7 @@
         <v>51</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2393,71 +2404,71 @@
         <v>56</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>294</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="D39" s="30" t="s">
         <v>298</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2470,8 +2481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6BCF3-52DA-45D5-A06F-31378179F4D8}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="K232" sqref="K232"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2703,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2796,10 +2807,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -2817,13 +2828,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2841,13 +2852,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
@@ -2869,7 +2880,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -2887,13 +2898,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -2911,13 +2922,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -2935,13 +2946,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D14" s="3">
         <v>10</v>
@@ -2959,13 +2970,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D15" s="3">
         <v>10</v>
@@ -2983,13 +2994,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D16" s="3">
         <v>10</v>
@@ -3007,13 +3018,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -3031,13 +3042,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
@@ -3055,13 +3066,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D19" s="3">
         <v>10</v>
@@ -3079,13 +3090,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D20" s="3">
         <v>10</v>
@@ -3521,13 +3532,13 @@
       <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D39">
@@ -3542,31 +3553,40 @@
       <c r="G39">
         <v>38</v>
       </c>
-      <c r="H39" s="24"/>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D40">
-        <v>10</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
+      <c r="A40" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D40" s="3">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
         <v>39</v>
       </c>
       <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="31" t="s">
         <v>28</v>
       </c>
       <c r="D41">
@@ -3581,7 +3601,7 @@
       <c r="G41">
         <v>40</v>
       </c>
-      <c r="H41" s="24"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
@@ -3798,7 +3818,7 @@
         <v>49</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,7 +4407,7 @@
       <c r="G76">
         <v>75</v>
       </c>
-      <c r="H76" s="33" t="s">
+      <c r="H76" s="35" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4413,7 +4433,7 @@
       <c r="G77" s="15">
         <v>76</v>
       </c>
-      <c r="H77" s="34"/>
+      <c r="H77" s="36"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -4437,7 +4457,7 @@
       <c r="G78">
         <v>77</v>
       </c>
-      <c r="H78" s="34"/>
+      <c r="H78" s="36"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
@@ -4471,7 +4491,7 @@
         <v>68</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D80">
         <v>10</v>
@@ -4618,13 +4638,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>299</v>
       </c>
       <c r="D87" s="3">
         <v>10</v>
@@ -6283,15 +6303,9 @@
       <c r="H160" s="24"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B161" s="9">
-        <v>5</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>151</v>
-      </c>
+      <c r="A161" s="3"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="8"/>
       <c r="D161">
         <v>10</v>
       </c>
@@ -6307,6 +6321,15 @@
       <c r="H161" s="24"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C162" t="s">
+        <v>304</v>
+      </c>
       <c r="D162">
         <v>10</v>
       </c>
@@ -6326,7 +6349,7 @@
         <v>15</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163">
@@ -6348,7 +6371,7 @@
         <v>6</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C164" s="16"/>
       <c r="D164" s="15">
@@ -6370,7 +6393,7 @@
         <v>19</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165">
@@ -6389,10 +6412,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166">
@@ -6414,7 +6437,7 @@
         <v>66</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167">
@@ -6436,7 +6459,7 @@
         <v>11</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168">
@@ -6491,7 +6514,7 @@
         <v>141</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D171">
         <v>10</v>
@@ -6515,7 +6538,7 @@
         <v>141</v>
       </c>
       <c r="C172" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D172" s="15">
         <v>10</v>
@@ -6539,7 +6562,7 @@
         <v>141</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D173">
         <v>10</v>
@@ -6563,7 +6586,7 @@
         <v>141</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D174">
         <v>10</v>
@@ -6602,7 +6625,7 @@
         <v>143</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D176">
         <v>10</v>
@@ -6626,7 +6649,7 @@
         <v>143</v>
       </c>
       <c r="C177" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D177" s="15">
         <v>10</v>
@@ -6650,7 +6673,7 @@
         <v>143</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D178">
         <v>10</v>
@@ -6674,7 +6697,7 @@
         <v>143</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D179">
         <v>10</v>
@@ -6698,7 +6721,7 @@
         <v>143</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D180">
         <v>10</v>
@@ -6722,7 +6745,7 @@
         <v>118</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D181">
         <v>10</v>
@@ -6746,7 +6769,7 @@
         <v>118</v>
       </c>
       <c r="C182" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D182" s="15">
         <v>10</v>
@@ -6770,7 +6793,7 @@
         <v>118</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D183">
         <v>10</v>
@@ -6794,7 +6817,7 @@
         <v>118</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D184">
         <v>10</v>
@@ -6818,7 +6841,7 @@
         <v>118</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D185">
         <v>10</v>
@@ -6842,7 +6865,7 @@
         <v>120</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D186">
         <v>10</v>
@@ -6866,7 +6889,7 @@
         <v>120</v>
       </c>
       <c r="C187" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D187" s="15">
         <v>10</v>
@@ -6890,7 +6913,7 @@
         <v>120</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D188">
         <v>10</v>
@@ -6914,7 +6937,7 @@
         <v>120</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D189">
         <v>10</v>
@@ -6938,7 +6961,7 @@
         <v>120</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D190">
         <v>10</v>
@@ -6962,7 +6985,7 @@
         <v>135</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D191">
         <v>10</v>
@@ -6986,7 +7009,7 @@
         <v>135</v>
       </c>
       <c r="C192" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D192" s="15">
         <v>10</v>
@@ -7010,7 +7033,7 @@
         <v>135</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D193">
         <v>10</v>
@@ -7034,7 +7057,7 @@
         <v>135</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D194">
         <v>10</v>
@@ -7073,7 +7096,7 @@
         <v>137</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D196">
         <v>10</v>
@@ -7097,7 +7120,7 @@
         <v>137</v>
       </c>
       <c r="C197" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D197" s="15">
         <v>10</v>
@@ -7121,7 +7144,7 @@
         <v>137</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D198">
         <v>10</v>
@@ -7145,7 +7168,7 @@
         <v>137</v>
       </c>
       <c r="C199" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D199">
         <v>10</v>
@@ -7184,7 +7207,7 @@
         <v>129</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D201">
         <v>10</v>
@@ -7208,7 +7231,7 @@
         <v>129</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D202" s="15">
         <v>10</v>
@@ -7232,7 +7255,7 @@
         <v>129</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D203">
         <v>10</v>
@@ -7256,7 +7279,7 @@
         <v>129</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D204">
         <v>10</v>
@@ -7295,7 +7318,7 @@
         <v>131</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D206">
         <v>10</v>
@@ -7319,7 +7342,7 @@
         <v>131</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D207" s="15">
         <v>10</v>
@@ -7343,7 +7366,7 @@
         <v>131</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D208">
         <v>10</v>
@@ -7367,7 +7390,7 @@
         <v>131</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D209">
         <v>10</v>
@@ -7387,11 +7410,11 @@
       <c r="A210" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B210" s="31" t="s">
-        <v>186</v>
+      <c r="B210" s="33" t="s">
+        <v>184</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D210">
         <v>10</v>
@@ -7406,16 +7429,16 @@
         <v>209</v>
       </c>
       <c r="H210" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B211" s="32"/>
+      <c r="B211" s="34"/>
       <c r="C211" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D211" s="15">
         <v>10</v>
@@ -7435,11 +7458,11 @@
       <c r="A212" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B212" s="31" t="s">
-        <v>190</v>
+      <c r="B212" s="33" t="s">
+        <v>188</v>
       </c>
       <c r="C212" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D212">
         <v>10</v>
@@ -7454,16 +7477,16 @@
         <v>211</v>
       </c>
       <c r="H212" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B213" s="32"/>
+      <c r="B213" s="34"/>
       <c r="C213" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D213" s="15">
         <v>10</v>
@@ -7483,11 +7506,11 @@
       <c r="A214" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B214" s="31" t="s">
-        <v>192</v>
+      <c r="B214" s="33" t="s">
+        <v>190</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D214">
         <v>10</v>
@@ -7502,16 +7525,16 @@
         <v>213</v>
       </c>
       <c r="H214" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B215" s="32"/>
+      <c r="B215" s="34"/>
       <c r="C215" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D215" s="15">
         <v>10</v>
@@ -7531,11 +7554,11 @@
       <c r="A216" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B216" s="31" t="s">
-        <v>194</v>
+      <c r="B216" s="33" t="s">
+        <v>192</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D216">
         <v>10</v>
@@ -7550,16 +7573,16 @@
         <v>215</v>
       </c>
       <c r="H216" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B217" s="32"/>
+      <c r="B217" s="34"/>
       <c r="C217" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D217" s="15">
         <v>10</v>
@@ -7579,11 +7602,11 @@
       <c r="A218" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B218" s="31" t="s">
-        <v>196</v>
+      <c r="B218" s="33" t="s">
+        <v>194</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D218">
         <v>10</v>
@@ -7598,16 +7621,16 @@
         <v>217</v>
       </c>
       <c r="H218" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B219" s="32"/>
+      <c r="B219" s="34"/>
       <c r="C219" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D219" s="15">
         <v>10</v>
@@ -7627,11 +7650,11 @@
       <c r="A220" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B220" s="31" t="s">
-        <v>198</v>
+      <c r="B220" s="33" t="s">
+        <v>196</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D220">
         <v>10</v>
@@ -7646,16 +7669,16 @@
         <v>219</v>
       </c>
       <c r="H220" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B221" s="32"/>
+      <c r="B221" s="34"/>
       <c r="C221" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D221" s="15">
         <v>10</v>
@@ -7675,11 +7698,11 @@
       <c r="A222" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B222" s="31" t="s">
-        <v>200</v>
+      <c r="B222" s="33" t="s">
+        <v>198</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D222">
         <v>10</v>
@@ -7694,16 +7717,16 @@
         <v>221</v>
       </c>
       <c r="H222" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B223" s="32"/>
+      <c r="B223" s="34"/>
       <c r="C223" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D223" s="15">
         <v>10</v>
@@ -7723,11 +7746,11 @@
       <c r="A224" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B224" s="31" t="s">
-        <v>202</v>
+      <c r="B224" s="33" t="s">
+        <v>200</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D224">
         <v>10</v>
@@ -7742,16 +7765,16 @@
         <v>223</v>
       </c>
       <c r="H224" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B225" s="32"/>
+      <c r="B225" s="34"/>
       <c r="C225" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D225" s="15">
         <v>10</v>
@@ -7784,11 +7807,11 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B227" s="3"/>
       <c r="C227" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D227" s="15">
         <v>10</v>
@@ -7806,11 +7829,11 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B228" s="3"/>
       <c r="C228" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D228" s="15">
         <v>10</v>
@@ -7828,11 +7851,11 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B229" s="3"/>
       <c r="C229" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D229" s="15">
         <v>10</v>
@@ -7868,7 +7891,7 @@
         <v>15</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3">
@@ -7890,7 +7913,7 @@
         <v>6</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C232" s="13"/>
       <c r="D232" s="13">
@@ -7912,7 +7935,7 @@
         <v>19</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="3">
@@ -7931,10 +7954,10 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3">
@@ -7956,7 +7979,7 @@
         <v>66</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3">
@@ -7978,7 +8001,7 @@
         <v>11</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3">
@@ -8015,7 +8038,7 @@
         <v>15</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3">
@@ -8037,7 +8060,7 @@
         <v>6</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C239" s="13"/>
       <c r="D239" s="13">
@@ -8059,7 +8082,7 @@
         <v>19</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3">
@@ -8078,10 +8101,10 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3">
@@ -8103,7 +8126,7 @@
         <v>66</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3">
@@ -8125,7 +8148,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3">
@@ -8147,7 +8170,7 @@
         <v>32</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3">
@@ -8166,7 +8189,7 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
@@ -8186,7 +8209,7 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
@@ -8206,7 +8229,7 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
@@ -8226,7 +8249,7 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
@@ -8246,7 +8269,7 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
@@ -8266,7 +8289,7 @@
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
@@ -8286,7 +8309,7 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
@@ -8366,7 +8389,7 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>

</xml_diff>